<commit_message>
Updates on the train/test notebooks
adjustments
</commit_message>
<xml_diff>
--- a/Accuracy Comparison.xlsx
+++ b/Accuracy Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j_ale\Documents\GitHub\img-processing-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947760A0-2D51-4FD7-8FC6-59BA1581D378}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E39E46-5791-4904-894F-B99E75646954}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9E210CB0-6B7E-4A81-93A6-484CDF5603B6}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -455,7 +455,7 @@
     <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="27.6">
+    <row r="2" spans="1:5">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>0.28776978417266103</v>
+        <v>0.28057553956834502</v>
       </c>
       <c r="C5" s="1">
-        <v>0.33093525179856098</v>
+        <v>0.36690647482014299</v>
       </c>
       <c r="D5" s="1">
         <v>0.16393442622950799</v>
@@ -536,5 +536,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>